<commit_message>
feature: add users by excel file
</commit_message>
<xml_diff>
--- a/Test-算法设计.xlsx
+++ b/Test-算法设计.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\PyCharm\workspace\exam-online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F1F38D-585B-4DBD-87FD-1B38C9445988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF013B-3B41-462D-A8A2-738BC6800DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7C737266-6D0A-418A-B993-2ECB4FBF5666}"/>
+    <workbookView xWindow="6144" yWindow="2160" windowWidth="17280" windowHeight="8964" xr2:uid="{7C737266-6D0A-418A-B993-2ECB4FBF5666}"/>
   </bookViews>
   <sheets>
     <sheet name="单项选择题" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,107 +84,217 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>我是多项选择题1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我是多项选择题2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我是多项选择题3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>判断题1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>T</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>判断题2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>判断题3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BCD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>判断题4</t>
-  </si>
-  <si>
-    <t>判断题5</t>
-  </si>
-  <si>
-    <t>题目0：答案是A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>题目1：答案是A</t>
-  </si>
-  <si>
-    <t>题目2：答案是A</t>
-  </si>
-  <si>
-    <t>题目3：答案是A</t>
-  </si>
-  <si>
-    <t>题目4：答案是A</t>
-  </si>
-  <si>
-    <t>题目5：答案是A</t>
-  </si>
-  <si>
-    <t>题目6：答案是A</t>
-  </si>
-  <si>
-    <t>题目7：答案是A</t>
-  </si>
-  <si>
-    <t>题目8：答案是A</t>
-  </si>
-  <si>
-    <t>题目9：答案是A</t>
-  </si>
-  <si>
-    <t>我是正确答案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我是错误答案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>我是多项选择题4</t>
-  </si>
-  <si>
     <t>BCD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>请简述最短路径算法，并证明之。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请简述堆排序算法的主要思想。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最短路径算法答案。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>堆排序算法答案</t>
+    <t>应用Johnson法则的流水作业调度采用的算法是</t>
+  </si>
+  <si>
+    <t>贪心算法</t>
+  </si>
+  <si>
+    <t>分支限界法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划算法的基本要素为</t>
+  </si>
+  <si>
+    <t>最优子结构性质与贪心选择性质</t>
+  </si>
+  <si>
+    <t>重叠子问题性质与贪心选择性质</t>
+  </si>
+  <si>
+    <t>最优子结构性质与重叠子问题性质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预排序与递归调用</t>
+  </si>
+  <si>
+    <t>能采用贪心算法求最优解的问题，一般具有的重要性质为：</t>
+  </si>
+  <si>
+    <t>重叠子问题性质与贪心选择性质 </t>
+  </si>
+  <si>
+    <t>最优子结构性质与重叠子问题性质 </t>
+  </si>
+  <si>
+    <t>预排序与递归调用 </t>
+  </si>
+  <si>
+    <t>回溯法在问题的解空间树中，按（）策略，从根结点出发搜索解空间树。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广度优先</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活结点优先</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扩展节点优先</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深度优先</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分支限界法在问题的解空间树中，按（）策略，从根结点出发搜索解空间树。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t> 回溯法的效率不依赖于以下哪一个因素？</t>
+  </si>
+  <si>
+    <t>产生x[k]的时间；</t>
+  </si>
+  <si>
+    <t>满足显约束的x[k]值的个数； </t>
+  </si>
+  <si>
+    <t>问题的解空间的形式；  </t>
+  </si>
+  <si>
+    <t>计算上界函数bound的时间；</t>
+  </si>
+  <si>
+    <t>常见的两种分支限界法为</t>
+  </si>
+  <si>
+    <t>广度优先分支限界法与深度优先分支限界法；</t>
+  </si>
+  <si>
+    <t>队列式（FIFO）分支限界法与堆栈式分支限界法； </t>
+  </si>
+  <si>
+    <t>排列树法与子集树法； </t>
+  </si>
+  <si>
+    <t>队列式（FIFO）分支限界法与优先队列式分支限界法； </t>
+  </si>
+  <si>
+    <t>k带图灵机的空间复杂性S(n)是指</t>
+  </si>
+  <si>
+    <t>k带图灵机处理所有长度为n的输入时，在某条带上所使用过的最大方格数。</t>
+  </si>
+  <si>
+    <t>k带图灵机处理所有长度为n的输入时，在k条带上所使用过的方格数的总和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k带图灵机处理所有长度为n的输入时，在k条带上所使用过的平均方格数。 </t>
+  </si>
+  <si>
+    <t>k带图灵机处理所有长度为n的输入时，在某条带上所使用过的最小方格数。</t>
+  </si>
+  <si>
+    <t>NP类语言在图灵机下的定义为</t>
+  </si>
+  <si>
+    <t>NP={L|L是一个能在非多项式时间内被一台NDTM所接受的语言}</t>
+  </si>
+  <si>
+    <t>NP={L|L是一个能在多项式时间内被一台NDTM所接受的语言}</t>
+  </si>
+  <si>
+    <t>NP={L|L是一个能在多项式时间内被一台DTM所接受的语言}</t>
+  </si>
+  <si>
+    <t>NP={L|L是一个能在多项式时间内被一台NDTM所接受的语言}；</t>
+  </si>
+  <si>
+    <t>试述回溯法的基本思想及用回溯法解题的步骤。</t>
+  </si>
+  <si>
+    <t>回溯算法答案。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简述归并排序算法和快速排序算法的分治方法。</t>
+  </si>
+  <si>
+    <t>归并与快排答案。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求最短路径可以使用什么算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prim算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dijkstra算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kruskal算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冒泡排序算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算法设计多项选择题1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算法设计多项选择题2</t>
+  </si>
+  <si>
+    <t>算法设计多项选择题3</t>
+  </si>
+  <si>
+    <t>算法设计多项选择题4</t>
+  </si>
+  <si>
+    <t>算法设计判断题1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算法设计判断题2</t>
+  </si>
+  <si>
+    <t>算法设计判断题3</t>
+  </si>
+  <si>
+    <t>算法设计判断题4</t>
+  </si>
+  <si>
+    <t>算法设计判断题5</t>
+  </si>
+  <si>
+    <t>F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -565,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A2D115-BB32-49B2-A3DD-40659F06ED1A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -600,22 +710,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2">
         <v>5</v>
@@ -623,22 +733,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
         <v>5</v>
@@ -646,22 +756,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2">
         <v>5</v>
@@ -669,22 +779,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2">
         <v>5</v>
@@ -692,22 +802,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -715,22 +825,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
@@ -738,22 +848,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G8" s="2">
         <v>5</v>
@@ -761,22 +871,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
         <v>5</v>
@@ -784,22 +894,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2">
         <v>5</v>
@@ -807,22 +917,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2">
         <v>5</v>
@@ -854,7 +964,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -888,7 +998,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -911,7 +1021,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -926,7 +1036,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
         <v>5</v>
@@ -934,7 +1044,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -957,7 +1067,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -972,7 +1082,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1">
         <v>5</v>
@@ -990,7 +1100,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1012,10 +1122,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -1023,10 +1133,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -1034,10 +1144,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1045,10 +1155,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1056,10 +1166,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1075,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0E2814-3D8F-4C70-A24C-B929CCD15FBE}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1094,10 +1204,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1105,10 +1215,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C3">
         <v>10</v>

</xml_diff>